<commit_message>
LAPR5-89 #report #implementation RGPD
</commit_message>
<xml_diff>
--- a/doc/Sprint B/rgpd/g051_rgpd.xlsx
+++ b/doc/Sprint B/rgpd/g051_rgpd.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866C5563-7C4E-4CFD-B444-19AAE4B2B4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2E1906-AA73-4EDE-8E67-3CEA9376D0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="histórico de alterações" sheetId="9" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="429">
   <si>
     <t>Nome</t>
   </si>
@@ -755,12 +755,6 @@
     <t>Versão</t>
   </si>
   <si>
-    <t>ex: 17/08/2018</t>
-  </si>
-  <si>
-    <t>ex: 1.0</t>
-  </si>
-  <si>
     <t>NIPC</t>
   </si>
   <si>
@@ -1106,9 +1100,6 @@
     <t>Outros</t>
   </si>
   <si>
-    <t>ex: funcionário teste</t>
-  </si>
-  <si>
     <t>NIF</t>
   </si>
   <si>
@@ -1157,9 +1148,6 @@
     <t>prazo de conservação</t>
   </si>
   <si>
-    <t>ex: 2, 3 e 5</t>
-  </si>
-  <si>
     <t>nome da entidade</t>
   </si>
   <si>
@@ -1311,6 +1299,21 @@
   </si>
   <si>
     <t>Consentimento do titular dos dados para o tratamento dos seus dados pessoais (Artigo 6º, nº1, alínea a)</t>
+  </si>
+  <si>
+    <t>1 e 2</t>
+  </si>
+  <si>
+    <t>Pedro Santos</t>
+  </si>
+  <si>
+    <t>Tiago Costa</t>
+  </si>
+  <si>
+    <t>Beatriz Seixas</t>
+  </si>
+  <si>
+    <t>Jéssica Alves</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1603,20 +1606,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1633,7 +1631,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,10 +1655,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1672,13 +1682,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -2023,7 +2027,9 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2041,43 +2047,67 @@
         <v>241</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>243</v>
+      <c r="A2" s="63">
+        <v>44517</v>
+      </c>
+      <c r="B2" s="23">
+        <v>1</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>359</v>
+        <v>425</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>376</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="63">
+        <v>44524</v>
+      </c>
+      <c r="B3" s="23">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="63">
+        <v>44531</v>
+      </c>
+      <c r="B4" s="23">
+        <v>3</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>427</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="63">
+        <v>44534</v>
+      </c>
+      <c r="B5" s="23">
+        <v>4</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>426</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -2348,26 +2378,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>253</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44"/>
+      <c r="A1" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="11" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B3" s="46"/>
+      <c r="A3" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" s="45"/>
       <c r="C3" s="11">
         <v>242818196</v>
       </c>
@@ -2380,7 +2410,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2398,32 +2428,32 @@
         <v>11</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="61" t="s">
-        <v>399</v>
+      <c r="B8" s="40"/>
+      <c r="C8" s="38" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="11">
         <v>987654321</v>
       </c>
@@ -2434,17 +2464,17 @@
       <c r="C10" s="35"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="37"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2473,45 +2503,45 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="31" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="37"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="37"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
-        <v>393</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="41" t="s">
+        <v>389</v>
+      </c>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B21" s="46"/>
+      <c r="A21" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21" s="45"/>
       <c r="C21" s="11">
         <v>253817307</v>
       </c>
@@ -2524,7 +2554,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2542,32 +2572,32 @@
         <v>11</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="61" t="s">
-        <v>404</v>
+      <c r="B26" s="40"/>
+      <c r="C26" s="38" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="11">
         <v>917654320</v>
       </c>
@@ -2578,26 +2608,26 @@
       <c r="C28" s="35"/>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
-        <v>393</v>
-      </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="41" t="s">
+        <v>389</v>
+      </c>
+      <c r="B29" s="42"/>
+      <c r="C29" s="43"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="38"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B31" s="46"/>
+      <c r="A31" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" s="45"/>
       <c r="C31" s="11">
         <v>281216312</v>
       </c>
@@ -2610,7 +2640,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,57 +2656,57 @@
         <v>11</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="13" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="61" t="s">
-        <v>405</v>
+      <c r="B36" s="40"/>
+      <c r="C36" s="38" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="38"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="11">
         <v>937654322</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="42" t="s">
-        <v>393</v>
-      </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="44"/>
+      <c r="A39" s="41" t="s">
+        <v>389</v>
+      </c>
+      <c r="B39" s="42"/>
+      <c r="C39" s="43"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="11" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B41" s="46"/>
+      <c r="A41" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="B41" s="45"/>
       <c r="C41" s="11">
         <v>278617263</v>
       </c>
@@ -2689,7 +2719,7 @@
         <v>9</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2707,57 +2737,57 @@
         <v>11</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="13" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="61" t="s">
-        <v>406</v>
+      <c r="B46" s="40"/>
+      <c r="C46" s="38" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="38"/>
+      <c r="B47" s="40"/>
       <c r="C47" s="11">
         <v>927654323</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="42" t="s">
-        <v>393</v>
-      </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="44"/>
+      <c r="A49" s="41" t="s">
+        <v>389</v>
+      </c>
+      <c r="B49" s="42"/>
+      <c r="C49" s="43"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="38"/>
+      <c r="B50" s="40"/>
       <c r="C50" s="11" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B51" s="46"/>
+      <c r="A51" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="B51" s="45"/>
       <c r="C51" s="11">
         <v>221568069</v>
       </c>
@@ -2770,7 +2800,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2788,54 +2818,52 @@
         <v>11</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="13" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="61" t="s">
-        <v>407</v>
+      <c r="B56" s="40"/>
+      <c r="C56" s="38" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
+      <c r="A57" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="38"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="11">
         <v>967654324</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A36:B36"/>
@@ -2845,15 +2873,17 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1" xr:uid="{3C28A1D8-EC5E-413E-9305-A95CC9994F69}"/>
@@ -2879,7 +2909,7 @@
   </sheetPr>
   <dimension ref="A1:AI103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:C2"/>
       <selection pane="topRight" sqref="A1:C2"/>
@@ -2910,182 +2940,182 @@
       <c r="A1" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
       <c r="AB1" s="30"/>
-      <c r="AC1" s="48" t="s">
-        <v>245</v>
-      </c>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
+      <c r="AC1" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
       <c r="AI1" s="51" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53" t="s">
+        <v>365</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53" t="s">
+        <v>366</v>
+      </c>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53" t="s">
         <v>367</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53" t="s">
         <v>368</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49" t="s">
+      <c r="N2" s="53"/>
+      <c r="O2" s="53" t="s">
         <v>369</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49" t="s">
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53" t="s">
         <v>370</v>
       </c>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49" t="s">
-        <v>371</v>
-      </c>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49" t="s">
-        <v>372</v>
-      </c>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49" t="s">
-        <v>373</v>
-      </c>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49" t="s">
+      <c r="R2" s="53"/>
+      <c r="S2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49" t="s">
-        <v>362</v>
-      </c>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49" t="s">
+      <c r="T2" s="53"/>
+      <c r="U2" s="53" t="s">
+        <v>359</v>
+      </c>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49" t="s">
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="47" t="s">
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="54" t="s">
+        <v>352</v>
+      </c>
+      <c r="AD2" s="53" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE2" s="53" t="s">
         <v>354</v>
       </c>
-      <c r="AD2" s="49" t="s">
+      <c r="AF2" s="53" t="s">
         <v>355</v>
       </c>
-      <c r="AE2" s="49" t="s">
+      <c r="AG2" s="52" t="s">
         <v>356</v>
       </c>
-      <c r="AF2" s="49" t="s">
-        <v>357</v>
-      </c>
-      <c r="AG2" s="48" t="s">
-        <v>358</v>
-      </c>
-      <c r="AH2" s="48"/>
+      <c r="AH2" s="52"/>
       <c r="AI2" s="51"/>
     </row>
     <row r="3" spans="1:35" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="50"/>
-      <c r="B3" s="49"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="R3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="S3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="U3" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="V3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="W3" s="29" t="s">
         <v>16</v>
@@ -3094,7 +3124,7 @@
         <v>17</v>
       </c>
       <c r="Y3" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Z3" s="29" t="s">
         <v>16</v>
@@ -3103,12 +3133,12 @@
         <v>17</v>
       </c>
       <c r="AB3" s="29" t="s">
-        <v>375</v>
-      </c>
-      <c r="AC3" s="47"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49"/>
+        <v>372</v>
+      </c>
+      <c r="AC3" s="54"/>
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53"/>
       <c r="AG3" s="29" t="s">
         <v>16</v>
       </c>
@@ -3122,60 +3152,60 @@
         <v>22</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="60"/>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="60"/>
-      <c r="Z4" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AA4" s="60"/>
-      <c r="AB4" s="60"/>
-      <c r="AC4" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD4" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE4" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF4" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG4" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AH4" s="60"/>
-      <c r="AI4" s="60" t="s">
-        <v>427</v>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD4" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE4" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF4" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG4" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="75" x14ac:dyDescent="0.25">
@@ -3183,64 +3213,64 @@
         <v>23</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37" t="s">
         <v>410</v>
       </c>
-      <c r="L5" s="25" t="s">
-        <v>408</v>
-      </c>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
-      <c r="V5" s="60"/>
-      <c r="W5" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="60"/>
-      <c r="Z5" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60"/>
-      <c r="AC5" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD5" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE5" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF5" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG5" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AH5" s="62"/>
-      <c r="AI5" s="60" t="s">
-        <v>427</v>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD5" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE5" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF5" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG5" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AH5" s="39"/>
+      <c r="AI5" s="37" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="75" x14ac:dyDescent="0.25">
@@ -3248,64 +3278,64 @@
         <v>24</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AA6" s="37"/>
+      <c r="AB6" s="37"/>
+      <c r="AC6" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD6" s="37" t="s">
         <v>411</v>
       </c>
-      <c r="J6" s="25" t="s">
-        <v>408</v>
-      </c>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="60"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="60"/>
-      <c r="W6" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="X6" s="60"/>
-      <c r="Y6" s="60"/>
-      <c r="Z6" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AA6" s="60"/>
-      <c r="AB6" s="60"/>
-      <c r="AC6" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD6" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE6" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF6" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG6" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AH6" s="60"/>
-      <c r="AI6" s="60" t="s">
-        <v>427</v>
+      <c r="AE6" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF6" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG6" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AH6" s="37"/>
+      <c r="AI6" s="37" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="75" x14ac:dyDescent="0.25">
@@ -3313,64 +3343,64 @@
         <v>25</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="60"/>
-      <c r="W7" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AA7" s="60"/>
-      <c r="AB7" s="60"/>
-      <c r="AC7" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD7" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE7" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF7" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG7" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AH7" s="60"/>
-      <c r="AI7" s="60" t="s">
-        <v>427</v>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AA7" s="37"/>
+      <c r="AB7" s="37"/>
+      <c r="AC7" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD7" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE7" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF7" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG7" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AH7" s="37"/>
+      <c r="AI7" s="37" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="60" x14ac:dyDescent="0.25">
@@ -3378,21 +3408,21 @@
         <v>26</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
@@ -3408,34 +3438,34 @@
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
       <c r="V8" s="16"/>
-      <c r="W8" s="60" t="s">
-        <v>414</v>
+      <c r="W8" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="X8" s="16"/>
       <c r="Y8" s="16"/>
-      <c r="Z8" s="60" t="s">
-        <v>414</v>
+      <c r="Z8" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AA8" s="16"/>
       <c r="AB8" s="16"/>
-      <c r="AC8" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD8" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE8" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF8" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG8" s="60" t="s">
-        <v>414</v>
+      <c r="AC8" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD8" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE8" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF8" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG8" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AH8" s="16"/>
       <c r="AI8" s="16" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="90" x14ac:dyDescent="0.25">
@@ -3443,13 +3473,13 @@
         <v>27</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
@@ -3469,34 +3499,34 @@
       <c r="T9" s="16"/>
       <c r="U9" s="16"/>
       <c r="V9" s="16"/>
-      <c r="W9" s="60" t="s">
-        <v>414</v>
+      <c r="W9" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="X9" s="16"/>
       <c r="Y9" s="16"/>
-      <c r="Z9" s="60" t="s">
-        <v>414</v>
+      <c r="Z9" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AA9" s="16"/>
       <c r="AB9" s="16"/>
-      <c r="AC9" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD9" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE9" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF9" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG9" s="60" t="s">
-        <v>414</v>
+      <c r="AC9" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD9" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE9" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF9" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG9" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AH9" s="16"/>
       <c r="AI9" s="16" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="60" x14ac:dyDescent="0.25">
@@ -3504,13 +3534,13 @@
         <v>28</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -3531,33 +3561,33 @@
       <c r="U10" s="16"/>
       <c r="V10" s="16"/>
       <c r="W10" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
       <c r="Z10" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AA10" s="16"/>
       <c r="AB10" s="16"/>
-      <c r="AC10" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD10" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE10" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF10" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG10" s="60" t="s">
-        <v>414</v>
+      <c r="AC10" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD10" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE10" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF10" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG10" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AH10" s="16"/>
       <c r="AI10" s="16" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="45" x14ac:dyDescent="0.25">
@@ -3565,13 +3595,13 @@
         <v>29</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -3588,41 +3618,41 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
       <c r="S11" s="22" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="T11" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="U11" s="16"/>
       <c r="V11" s="16"/>
       <c r="W11" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="X11" s="16"/>
       <c r="Y11" s="16"/>
       <c r="Z11" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
-      <c r="AC11" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD11" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE11" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF11" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG11" s="60" t="s">
-        <v>414</v>
+      <c r="AC11" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD11" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE11" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF11" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG11" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AH11" s="16"/>
       <c r="AI11" s="16" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="45" x14ac:dyDescent="0.25">
@@ -3630,13 +3660,13 @@
         <v>30</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -3653,41 +3683,41 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="22" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="T12" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="U12" s="16"/>
       <c r="V12" s="16"/>
       <c r="W12" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="X12" s="16"/>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AA12" s="16"/>
       <c r="AB12" s="16"/>
-      <c r="AC12" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD12" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE12" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF12" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG12" s="60" t="s">
-        <v>414</v>
+      <c r="AC12" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD12" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE12" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF12" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG12" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AH12" s="16"/>
       <c r="AI12" s="16" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="45" x14ac:dyDescent="0.25">
@@ -3695,13 +3725,13 @@
         <v>31</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -3718,41 +3748,41 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
       <c r="S13" s="22" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="U13" s="16"/>
       <c r="V13" s="16"/>
       <c r="W13" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="X13" s="16"/>
       <c r="Y13" s="16"/>
       <c r="Z13" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AA13" s="16"/>
       <c r="AB13" s="16"/>
-      <c r="AC13" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AD13" s="60" t="s">
-        <v>415</v>
-      </c>
-      <c r="AE13" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AF13" s="60" t="s">
-        <v>414</v>
-      </c>
-      <c r="AG13" s="60" t="s">
-        <v>414</v>
+      <c r="AC13" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD13" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE13" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF13" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG13" s="37" t="s">
+        <v>410</v>
       </c>
       <c r="AH13" s="16"/>
       <c r="AI13" s="16" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -7267,6 +7297,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="AI1:AI3"/>
     <mergeCell ref="AC1:AH1"/>
@@ -7283,12 +7319,6 @@
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="AE2:AE3"/>
     <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="sim ou não" error="apenas estes dois valores são admitidos" sqref="W4:W103 Z4:Z103 AC4:AG103" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -7296,7 +7326,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="72" fitToWidth="4" fitToHeight="4" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" fitToWidth="4" fitToHeight="4" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F (folha &amp;A)</oddHeader>
     <oddFooter>&amp;L&amp;D  &amp;T&amp;R&amp;P/&amp;N</oddFooter>
@@ -7334,25 +7364,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>379</v>
-      </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="56" t="s">
+        <v>374</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>376</v>
+      </c>
+      <c r="G1" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="F1" s="53" t="s">
-        <v>380</v>
-      </c>
-      <c r="G1" s="55" t="s">
-        <v>382</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>365</v>
+      <c r="H1" s="58" t="s">
+        <v>362</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -7365,20 +7395,20 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
+      <c r="A2" s="55"/>
       <c r="B2" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>360</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -7391,26 +7421,26 @@
     </row>
     <row r="3" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="21" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -7424,24 +7454,24 @@
     </row>
     <row r="4" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="21" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -7455,7 +7485,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -7467,7 +7497,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -7479,7 +7509,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -7491,7 +7521,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -7503,7 +7533,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -7515,7 +7545,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -7527,7 +7557,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -7539,7 +7569,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -7551,7 +7581,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -7563,7 +7593,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
@@ -7575,7 +7605,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
@@ -7587,7 +7617,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -7599,7 +7629,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -7611,7 +7641,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -7623,7 +7653,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -7635,7 +7665,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -7647,7 +7677,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -7659,7 +7689,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -7671,7 +7701,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -7683,7 +7713,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -7695,7 +7725,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -7707,7 +7737,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
@@ -7719,7 +7749,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -7731,7 +7761,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
@@ -7743,7 +7773,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
@@ -7755,7 +7785,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
@@ -7767,7 +7797,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
@@ -7779,7 +7809,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -7791,7 +7821,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
@@ -7803,7 +7833,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
@@ -7815,7 +7845,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
@@ -7827,7 +7857,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
@@ -7839,7 +7869,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
@@ -7851,7 +7881,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
@@ -7863,7 +7893,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
@@ -7875,7 +7905,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
@@ -7887,7 +7917,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
@@ -7899,7 +7929,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
@@ -7911,7 +7941,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
@@ -7923,7 +7953,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B44" s="26"/>
       <c r="C44" s="26"/>
@@ -7935,7 +7965,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
@@ -7947,7 +7977,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>
@@ -7959,7 +7989,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="26"/>
@@ -7971,7 +8001,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
@@ -7983,7 +8013,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="26"/>
@@ -7995,7 +8025,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="26"/>
@@ -8007,7 +8037,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
@@ -8019,7 +8049,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B52" s="26"/>
       <c r="C52" s="26"/>
@@ -8031,7 +8061,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="26"/>
@@ -8043,7 +8073,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B54" s="26"/>
       <c r="C54" s="26"/>
@@ -8055,7 +8085,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B55" s="26"/>
       <c r="C55" s="26"/>
@@ -8067,7 +8097,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B56" s="26"/>
       <c r="C56" s="26"/>
@@ -8079,7 +8109,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B57" s="26"/>
       <c r="C57" s="26"/>
@@ -8091,7 +8121,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B58" s="26"/>
       <c r="C58" s="26"/>
@@ -8103,7 +8133,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B59" s="26"/>
       <c r="C59" s="26"/>
@@ -8115,7 +8145,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B60" s="26"/>
       <c r="C60" s="26"/>
@@ -8127,7 +8157,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B61" s="26"/>
       <c r="C61" s="26"/>
@@ -8139,7 +8169,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B62" s="26"/>
       <c r="C62" s="26"/>
@@ -8151,7 +8181,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B63" s="26"/>
       <c r="C63" s="26"/>
@@ -8163,7 +8193,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B64" s="26"/>
       <c r="C64" s="26"/>
@@ -8175,7 +8205,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B65" s="26"/>
       <c r="C65" s="26"/>
@@ -8187,7 +8217,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B66" s="26"/>
       <c r="C66" s="26"/>
@@ -8199,7 +8229,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B67" s="26"/>
       <c r="C67" s="26"/>
@@ -8211,7 +8241,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B68" s="26"/>
       <c r="C68" s="26"/>
@@ -8223,7 +8253,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B69" s="26"/>
       <c r="C69" s="26"/>
@@ -8235,7 +8265,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B70" s="26"/>
       <c r="C70" s="26"/>
@@ -8247,7 +8277,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="28" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B71" s="26"/>
       <c r="C71" s="26"/>
@@ -8259,7 +8289,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B72" s="26"/>
       <c r="C72" s="26"/>
@@ -8271,7 +8301,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="28" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B73" s="26"/>
       <c r="C73" s="26"/>
@@ -8283,7 +8313,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="28" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B74" s="26"/>
       <c r="C74" s="26"/>
@@ -8295,7 +8325,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="28" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B75" s="26"/>
       <c r="C75" s="26"/>
@@ -8307,7 +8337,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B76" s="26"/>
       <c r="C76" s="26"/>
@@ -8319,7 +8349,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B77" s="26"/>
       <c r="C77" s="26"/>
@@ -8331,7 +8361,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B78" s="26"/>
       <c r="C78" s="26"/>
@@ -8343,7 +8373,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="28" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B79" s="26"/>
       <c r="C79" s="26"/>
@@ -8355,7 +8385,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="28" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B80" s="26"/>
       <c r="C80" s="26"/>
@@ -8367,7 +8397,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B81" s="26"/>
       <c r="C81" s="26"/>
@@ -8379,7 +8409,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="28" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B82" s="26"/>
       <c r="C82" s="26"/>
@@ -8391,7 +8421,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B83" s="26"/>
       <c r="C83" s="26"/>
@@ -8403,7 +8433,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B84" s="26"/>
       <c r="C84" s="26"/>
@@ -8415,7 +8445,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B85" s="26"/>
       <c r="C85" s="26"/>
@@ -8427,7 +8457,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B86" s="26"/>
       <c r="C86" s="26"/>
@@ -8439,7 +8469,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B87" s="26"/>
       <c r="C87" s="26"/>
@@ -8451,7 +8481,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B88" s="26"/>
       <c r="C88" s="26"/>
@@ -8463,7 +8493,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B89" s="26"/>
       <c r="C89" s="26"/>
@@ -8475,7 +8505,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B90" s="26"/>
       <c r="C90" s="26"/>
@@ -8487,7 +8517,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="26"/>
@@ -8499,7 +8529,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B92" s="26"/>
       <c r="C92" s="26"/>
@@ -8511,7 +8541,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B93" s="26"/>
       <c r="C93" s="26"/>
@@ -8523,7 +8553,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B94" s="26"/>
       <c r="C94" s="26"/>
@@ -8535,7 +8565,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B95" s="26"/>
       <c r="C95" s="26"/>
@@ -8547,7 +8577,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="28" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B96" s="26"/>
       <c r="C96" s="26"/>
@@ -8559,7 +8589,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="28" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B97" s="26"/>
       <c r="C97" s="26"/>
@@ -8571,7 +8601,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="28" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B98" s="26"/>
       <c r="C98" s="26"/>
@@ -8583,7 +8613,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="28" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B99" s="26"/>
       <c r="C99" s="26"/>
@@ -8595,7 +8625,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="28" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B100" s="26"/>
       <c r="C100" s="26"/>
@@ -8607,7 +8637,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="28" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B101" s="26"/>
       <c r="C101" s="26"/>
@@ -8619,7 +8649,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="28" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B102" s="26"/>
       <c r="C102" s="26"/>
@@ -8631,7 +8661,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="28" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B103" s="26"/>
       <c r="C103" s="26"/>
@@ -8643,7 +8673,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="28" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B104" s="26"/>
       <c r="C104" s="26"/>
@@ -8722,7 +8752,7 @@
         <v>222</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>223</v>
@@ -8740,7 +8770,7 @@
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -8792,19 +8822,19 @@
     </row>
     <row r="6" spans="1:5" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="D6" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="21" t="s">
         <v>249</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>